<commit_message>
Se añade en la pestaña de of1Postscore los campos de ref
</commit_message>
<xml_diff>
--- a/UsoDatosBlaze.xlsx
+++ b/UsoDatosBlaze.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ovalencia\Documents\Documentación FO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222B815A-96BD-42F7-B2EC-FE693494CAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13AE83D-7FB2-489D-9015-0736F4DEF171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{1A68E9D1-20FD-463D-94C6-453385F048B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{1A68E9D1-20FD-463D-94C6-453385F048B6}"/>
   </bookViews>
   <sheets>
     <sheet name="of1Prescore" sheetId="3" r:id="rId1"/>
-    <sheet name="calculosIniciales" sheetId="2" r:id="rId2"/>
-    <sheet name="of2PrescoreTit" sheetId="4" r:id="rId3"/>
-    <sheet name="of1Postscore" sheetId="5" r:id="rId4"/>
+    <sheet name="of1Postscore" sheetId="5" r:id="rId2"/>
+    <sheet name="calculosIniciales" sheetId="2" r:id="rId3"/>
+    <sheet name="of2PrescoreTit" sheetId="4" r:id="rId4"/>
     <sheet name="Hoja5" sheetId="1" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_AMO_UniqueIdentifier" hidden="1">"'7c783109-3e0c-4d8c-99cb-68ada84179e1'"</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">calculosIniciales!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">calculosIniciales!$A$1:$M$33</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">of1Prescore!$A$1:$K$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">of2PrescoreTit!$A$1:$K$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">of2PrescoreTit!$A$1:$K$70</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27503" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27516" uniqueCount="180">
   <si>
     <t>Tipo Blaze</t>
   </si>
@@ -1019,7 +1019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABEE34B-3257-4FDE-A988-67278A5AD02D}">
   <dimension ref="A1:XFD20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -83013,6 +83013,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197E3104-B4B1-498D-BEEF-0D5E9BADC956}">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AA78C3F-A8DB-4245-947A-0DEEE20A9049}">
   <dimension ref="A1:M33"/>
   <sheetViews>
@@ -84081,7 +84152,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77664239-DF4C-4E9E-BABD-FF6E31D0CD2A}">
   <dimension ref="A1:M70"/>
   <sheetViews>
@@ -86050,20 +86121,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197E3104-B4B1-498D-BEEF-0D5E9BADC956}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2978C9A-3CE4-485F-A68E-0B12DA39F655}">
   <dimension ref="A1:B12"/>
@@ -86161,6 +86218,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f47d23a3-c7f1-4fff-865f-fdc022acaa51" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4d3be4-06a2-4534-ad05-af0e517b383e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100704F237149770645ADFBBB4BE52A6737" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="b8d40168d3b50169b0ae0e3a33d49c44">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4d3be4-06a2-4534-ad05-af0e517b383e" xmlns:ns3="f47d23a3-c7f1-4fff-865f-fdc022acaa51" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="377ac4a97eb5a6db26d34dbe58ff6bcd" ns2:_="" ns3:_="">
     <xsd:import namespace="6f4d3be4-06a2-4534-ad05-af0e517b383e"/>
@@ -86371,27 +86448,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f47d23a3-c7f1-4fff-865f-fdc022acaa51" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4d3be4-06a2-4534-ad05-af0e517b383e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1A39B34-F4F6-40ED-AB99-52CE9D73FDDE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{033D9230-47F6-4E9E-A248-0692A3164F77}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f47d23a3-c7f1-4fff-865f-fdc022acaa51"/>
+    <ds:schemaRef ds:uri="6f4d3be4-06a2-4534-ad05-af0e517b383e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C9455F0-0EF2-4B6F-A84A-6FD970207BD1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -86408,23 +86484,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{033D9230-47F6-4E9E-A248-0692A3164F77}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f47d23a3-c7f1-4fff-865f-fdc022acaa51"/>
-    <ds:schemaRef ds:uri="6f4d3be4-06a2-4534-ad05-af0e517b383e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1A39B34-F4F6-40ED-AB99-52CE9D73FDDE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>